<commit_message>
add mock csv data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/zakariae_belkassem_atos_net/Documents/Bureau/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atos365-my.sharepoint.com/personal/zakariae_belkassem_atos_net/Documents/Bureau/pfe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{DA30C52B-4F55-4E2F-BE70-A13D395A5D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50071608-87A2-4211-9003-B43027ED1152}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{DA30C52B-4F55-4E2F-BE70-A13D395A5D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1043D583-6952-4C9A-AE0B-2C55943691B6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F23659F4-64A2-48AB-903C-3CC724D0E1B4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="448">
   <si>
     <t>id</t>
   </si>
@@ -598,9 +598,6 @@
     <t>001-332-897-4722x4778</t>
   </si>
   <si>
-    <t>1972-08-08</t>
-  </si>
-  <si>
     <t>1972-07-24</t>
   </si>
   <si>
@@ -619,9 +616,6 @@
     <t>896.268.8348</t>
   </si>
   <si>
-    <t>1991-05-19</t>
-  </si>
-  <si>
     <t>1995-06-07</t>
   </si>
   <si>
@@ -658,9 +652,6 @@
     <t>649-266-2304</t>
   </si>
   <si>
-    <t>1983-06-18</t>
-  </si>
-  <si>
     <t>1999-07-08</t>
   </si>
   <si>
@@ -679,9 +670,6 @@
     <t>716.770.5283</t>
   </si>
   <si>
-    <t>1986-02-13</t>
-  </si>
-  <si>
     <t>2019-06-09</t>
   </si>
   <si>
@@ -700,9 +688,6 @@
     <t>771.735.4046x89836</t>
   </si>
   <si>
-    <t>1973-12-03</t>
-  </si>
-  <si>
     <t>1996-09-19</t>
   </si>
   <si>
@@ -721,9 +706,6 @@
     <t>001-414-527-3147x764</t>
   </si>
   <si>
-    <t>1976-01-06</t>
-  </si>
-  <si>
     <t>2017-08-24</t>
   </si>
   <si>
@@ -742,9 +724,6 @@
     <t>+1-592-367-1555x7806</t>
   </si>
   <si>
-    <t>1985-07-20</t>
-  </si>
-  <si>
     <t>1973-01-24</t>
   </si>
   <si>
@@ -763,9 +742,6 @@
     <t>001-697-918-3977x6465</t>
   </si>
   <si>
-    <t>1985-08-02</t>
-  </si>
-  <si>
     <t>2020-01-13</t>
   </si>
   <si>
@@ -784,9 +760,6 @@
     <t>001-394-216-4868</t>
   </si>
   <si>
-    <t>1983-02-06</t>
-  </si>
-  <si>
     <t>1995-09-18</t>
   </si>
   <si>
@@ -805,9 +778,6 @@
     <t>001-997-890-2420x631</t>
   </si>
   <si>
-    <t>1998-08-05</t>
-  </si>
-  <si>
     <t>2020-03-18</t>
   </si>
   <si>
@@ -826,9 +796,6 @@
     <t>+1-408-819-0837x850</t>
   </si>
   <si>
-    <t>2015-07-17</t>
-  </si>
-  <si>
     <t>1986-02-27</t>
   </si>
   <si>
@@ -844,9 +811,6 @@
     <t>001-908-687-6585</t>
   </si>
   <si>
-    <t>2021-12-07</t>
-  </si>
-  <si>
     <t>1990-12-27</t>
   </si>
   <si>
@@ -865,9 +829,6 @@
     <t>2436551969</t>
   </si>
   <si>
-    <t>2025-04-16</t>
-  </si>
-  <si>
     <t>2004-05-30</t>
   </si>
   <si>
@@ -886,9 +847,6 @@
     <t>681.751.6695</t>
   </si>
   <si>
-    <t>2006-07-31</t>
-  </si>
-  <si>
     <t>1984-10-07</t>
   </si>
   <si>
@@ -907,9 +865,6 @@
     <t>5339692969</t>
   </si>
   <si>
-    <t>1987-05-26</t>
-  </si>
-  <si>
     <t>1993-06-20</t>
   </si>
   <si>
@@ -925,9 +880,6 @@
     <t>001-764-338-0896x1030</t>
   </si>
   <si>
-    <t>1977-01-28</t>
-  </si>
-  <si>
     <t>1970-01-22</t>
   </si>
   <si>
@@ -946,9 +898,6 @@
     <t>566-579-5144</t>
   </si>
   <si>
-    <t>1995-01-23</t>
-  </si>
-  <si>
     <t>2015-09-28</t>
   </si>
   <si>
@@ -967,9 +916,6 @@
     <t>244.979.8221</t>
   </si>
   <si>
-    <t>1972-11-27</t>
-  </si>
-  <si>
     <t>2010-08-22</t>
   </si>
   <si>
@@ -988,9 +934,6 @@
     <t>3516635962</t>
   </si>
   <si>
-    <t>1996-12-12</t>
-  </si>
-  <si>
     <t>2004-05-25</t>
   </si>
   <si>
@@ -1009,9 +952,6 @@
     <t>329.459.9493x953</t>
   </si>
   <si>
-    <t>2011-07-16</t>
-  </si>
-  <si>
     <t>2015-06-13</t>
   </si>
   <si>
@@ -1030,9 +970,6 @@
     <t>698.318.3972x3985</t>
   </si>
   <si>
-    <t>1982-11-25</t>
-  </si>
-  <si>
     <t>2008-05-21</t>
   </si>
   <si>
@@ -1051,9 +988,6 @@
     <t>+1-374-963-4786x3200</t>
   </si>
   <si>
-    <t>1979-12-30</t>
-  </si>
-  <si>
     <t>2019-02-25</t>
   </si>
   <si>
@@ -1067,13 +1001,394 @@
   </si>
   <si>
     <t>West James</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3201</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3202</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3203</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3204</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3205</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3206</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3207</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3208</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3209</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3210</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3211</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3212</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3213</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3214</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3215</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3216</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3217</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3218</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3219</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3220</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3221</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3222</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3223</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3224</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3225</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3226</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3227</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3228</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3229</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3230</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3231</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3232</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3233</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3234</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3235</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3236</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3237</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3238</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3239</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3240</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3241</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3242</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3243</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3244</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3245</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3246</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3247</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3248</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3249</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3250</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3251</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3252</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3253</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3254</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3255</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3256</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3257</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3258</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3259</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3260</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3261</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3262</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3263</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3264</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3265</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3266</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3267</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3268</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3269</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3270</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3271</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3272</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3273</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3274</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3275</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3276</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3277</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3278</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3279</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3280</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3281</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3282</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3283</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3284</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3285</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3286</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3287</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3288</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3289</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3290</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3291</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3292</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3293</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3294</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3295</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3296</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3297</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3298</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3299</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3300</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3301</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3302</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3303</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3304</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3305</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3306</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3307</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3308</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3309</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3310</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3311</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3312</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3313</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3314</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3315</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3316</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3317</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3318</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3319</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3320</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3321</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3322</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3323</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3324</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3325</t>
+  </si>
+  <si>
+    <t>+1-374-963-4786x3326</t>
+  </si>
+  <si>
+    <t>12/31/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1088,6 +1403,16 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1104,7 +1429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1127,11 +1452,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF666666"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF666666"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF666666"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF666666"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1139,6 +1479,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1154,6 +1498,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1476,10 +1824,10 @@
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="2.90625" customWidth="1"/>
     <col min="2" max="2" width="21.81640625" customWidth="1"/>
@@ -1490,7 +1838,7 @@
     <col min="8" max="8" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1538,7 +1886,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1551,7 +1899,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1564,7 +1912,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1577,7 +1925,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1590,7 +1938,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1603,7 +1951,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1616,7 +1964,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1629,7 +1977,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1642,7 +1990,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1655,7 +2003,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1668,7 +2016,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1681,7 +2029,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1694,7 +2042,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1707,7 +2055,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1720,7 +2068,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1733,7 +2081,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1746,7 +2094,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1759,7 +2107,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1772,7 +2120,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1785,7 +2133,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1798,7 +2146,7 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1811,7 +2159,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1824,7 +2172,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1837,7 +2185,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1850,7 +2198,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1863,7 +2211,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1876,7 +2224,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1889,7 +2237,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1902,7 +2250,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1915,7 +2263,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1928,7 +2276,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1941,7 +2289,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1954,7 +2302,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1967,7 +2315,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1980,7 +2328,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1993,7 +2341,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2006,7 +2354,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2019,7 +2367,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2032,7 +2380,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2045,7 +2393,7 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2058,7 +2406,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2071,7 +2419,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2084,7 +2432,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2097,7 +2445,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2110,7 +2458,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2123,7 +2471,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2136,7 +2484,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2149,7 +2497,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2162,7 +2510,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2175,7 +2523,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2188,7 +2536,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2201,7 +2549,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2214,7 +2562,7 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2227,7 +2575,7 @@
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2240,7 +2588,7 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2253,7 +2601,7 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -2266,7 +2614,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -2279,7 +2627,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -2300,13 +2648,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152CE98A-2733-4A1C-8582-189CD93EBA0C}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5.08984375" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" customWidth="1"/>
@@ -2321,7 +2669,7 @@
     <col min="11" max="11" width="26.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2356,7 +2704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15" thickBot="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2366,23 +2714,23 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5">
+        <v>43831</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>23</v>
@@ -2391,33 +2739,33 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="15" thickBot="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>23</v>
@@ -2426,33 +2774,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>3</v>
@@ -2461,33 +2807,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>23</v>
@@ -2496,33 +2840,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>3</v>
@@ -2531,33 +2873,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>3</v>
@@ -2566,33 +2906,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>227</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>3</v>
@@ -2601,33 +2939,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>234</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>23</v>
@@ -2636,33 +2972,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>241</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>3</v>
@@ -2671,33 +3005,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>248</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>3</v>
@@ -2706,33 +3038,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>255</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>23</v>
@@ -2741,33 +3071,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>262</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>160</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>23</v>
@@ -2776,33 +3104,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>268</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>23</v>
@@ -2811,33 +3137,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>275</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>3</v>
@@ -2846,33 +3170,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>282</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>3</v>
@@ -2881,33 +3203,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>289</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>23</v>
@@ -2916,33 +3236,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>295</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>3</v>
@@ -2951,33 +3269,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>302</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>23</v>
@@ -2986,33 +3302,31 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>309</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>3</v>
@@ -3021,33 +3335,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>316</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>3</v>
@@ -3056,33 +3368,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>323</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>3</v>
@@ -3091,33 +3401,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>330</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>3</v>
@@ -3126,33 +3434,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>337</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>342</v>
+        <v>320</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>3</v>
@@ -3161,7 +3467,1395 @@
         <v>7</v>
       </c>
     </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2">
+        <v>84</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2">
+        <v>88</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2">
+        <v>90</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2">
+        <v>91</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
+        <v>92</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2">
+        <v>93</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2">
+        <v>94</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2">
+        <v>95</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="2">
+        <v>96</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="2">
+        <v>97</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="2">
+        <v>98</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2">
+        <v>102</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2">
+        <v>103</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2">
+        <v>104</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="2">
+        <v>105</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="2">
+        <v>126</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="2">
+        <v>127</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="2">
+        <v>128</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="2">
+        <v>129</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="2">
+        <v>130</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="2">
+        <v>131</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="2">
+        <v>132</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="2">
+        <v>134</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="2">
+        <v>135</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2">
+        <v>137</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2">
+        <v>138</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="2">
+        <v>139</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="2">
+        <v>140</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="2">
+        <v>141</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="2">
+        <v>142</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="2">
+        <v>143</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="2">
+        <v>144</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="2">
+        <v>145</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="2">
+        <v>146</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="2">
+        <v>147</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="2">
+        <v>148</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="2">
+        <v>149</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3174,7 +4868,7 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="19.81640625" customWidth="1"/>
     <col min="3" max="3" width="13.453125" customWidth="1"/>
@@ -3188,7 +4882,7 @@
     <col min="11" max="11" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3223,7 +4917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3258,7 +4952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3293,7 +4987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3328,7 +5022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3363,7 +5057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3398,7 +5092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3433,7 +5127,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3468,7 +5162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3503,7 +5197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3538,7 +5232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3573,7 +5267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3608,7 +5302,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3643,7 +5337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3678,7 +5372,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3713,7 +5407,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3748,7 +5442,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3783,7 +5477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3818,7 +5512,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3853,7 +5547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3888,7 +5582,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3923,7 +5617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3958,7 +5652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3993,7 +5687,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="2">
         <v>23</v>
       </c>

</xml_diff>